<commit_message>
working weather Api excluding QA
</commit_message>
<xml_diff>
--- a/src/main/resources/files/cities.xlsx
+++ b/src/main/resources/files/cities.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03979839-CF65-41C7-8DEB-5A8BA35D8DED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cities" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -31,12 +32,21 @@
   </si>
   <si>
     <t>Abuja</t>
+  </si>
+  <si>
+    <t>Manitoba</t>
+  </si>
+  <si>
+    <t>Ikeja</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,11 +357,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,6 +386,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
resolved white spaces in cities
</commit_message>
<xml_diff>
--- a/src/main/resources/files/cities.xlsx
+++ b/src/main/resources/files/cities.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D906BC5C-13BC-4A7C-9011-7F5E2ADA2946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4808014-FD5D-4779-940C-1698059EF5C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A2" sqref="A2:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Degree Symbol in email notification
</commit_message>
<xml_diff>
--- a/src/main/resources/files/cities.xlsx
+++ b/src/main/resources/files/cities.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4808014-FD5D-4779-940C-1698059EF5C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D906BC5C-13BC-4A7C-9011-7F5E2ADA2946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A101"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Auto stash before revert of "Merge branch 'test' into kene"
</commit_message>
<xml_diff>
--- a/src/main/resources/files/cities.xlsx
+++ b/src/main/resources/files/cities.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D906BC5C-13BC-4A7C-9011-7F5E2ADA2946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4808014-FD5D-4779-940C-1698059EF5C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A2" sqref="A2:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>